<commit_message>
default view now updated to main cover page
</commit_message>
<xml_diff>
--- a/Data/2025-05-29 Public Bodies Directory 2023_24.xlsx
+++ b/Data/2025-05-29 Public Bodies Directory 2023_24.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin.ingram/Martin Ingram R Work/23-24-Landscape-Analysis/Data Processing Pipeline/Final Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin.ingram/Martin Ingram R Work/ALB_Landscape_Analysis_2023_24/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BB77F4-43EB-2C41-A2B2-A13DB26951D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D7D899-CD7B-D04D-9018-05F070F12FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -7818,24 +7818,28 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -8362,7 +8366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -51603,7 +51607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>